<commit_message>
Added formatting for date,time,pct
</commit_message>
<xml_diff>
--- a/test/data/Types.xlsx
+++ b/test/data/Types.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10710"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10907"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kay/Sources/bb-excel/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D7AEFF-A834-5D40-A3BC-3A594DDAACE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B9167F-715F-2141-9A7E-7186AE0101D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="23820" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{BF774B14-1153-0A4D-A439-A114131FA868}"/>
+    <workbookView xWindow="6500" yWindow="2220" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{BF774B14-1153-0A4D-A439-A114131FA868}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Kay" sheetId="2" r:id="rId2"/>
+    <sheet name="Kay" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,11 +43,18 @@
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="1">
+  <futureMetadata name="XLRICHVALUE" count="2">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
         </ext>
       </extLst>
     </bk>
@@ -65,16 +73,19 @@
       <rc t="2" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="1">
+  <valueMetadata count="2">
     <bk>
       <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="50">
   <si>
     <t>Row</t>
   </si>
@@ -242,16 +253,28 @@
     <t>bbexcel</t>
   </si>
   <si>
-    <t>missing!</t>
-  </si>
-  <si>
-    <t>formatting</t>
-  </si>
-  <si>
     <t>(555) 608-5136</t>
   </si>
   <si>
     <t>Peanut Butter</t>
+  </si>
+  <si>
+    <t>formatting D</t>
+  </si>
+  <si>
+    <t>formatting D,E</t>
+  </si>
+  <si>
+    <t>formatting E</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t>Spill</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -293,7 +316,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +326,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,7 +350,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -350,8 +379,16 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -412,18 +449,30 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
   <rv s="0">
     <v>2</v>
     <v>1</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>8</v>
+    <v>0</v>
+    <v>3</v>
   </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
   <s t="_error">
     <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+  <s t="_error">
+    <k n="colOffset" t="i"/>
+    <k n="errorType" t="i"/>
+    <k n="rwOffset" t="i"/>
     <k n="subType" t="i"/>
   </s>
 </rvStructures>
@@ -725,11 +774,1026 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA93BC24-192B-C24A-B2B9-6C19BFA160A2}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="19">
+        <v>123456789.89</v>
+      </c>
+      <c r="E2">
+        <v>0.01</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>150</v>
+      </c>
+      <c r="E3">
+        <v>2.22333444555666E+20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="20">
+        <v>0.12</v>
+      </c>
+      <c r="E4" s="21">
+        <v>0.13399</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>1234.5689</v>
+      </c>
+      <c r="E5">
+        <v>-2.0000000000000001E-4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="22">
+        <v>44652</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="24">
+        <v>0.80233796296296289</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0.52708333333333335</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>-890</v>
+      </c>
+      <c r="E8">
+        <v>-9800</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="13">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="13">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="26">
+        <v>44562</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="13">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="27">
+        <v>0.17708333333333334</v>
+      </c>
+      <c r="F12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="13">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="b">
+        <f>IF(5=25/5,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="E13" t="b">
+        <f>"A"="A"</f>
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="13">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="b">
+        <f>0="A"</f>
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="13">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="e" cm="1">
+        <f t="array" aca="1" ref="D15" ca="1">su(A11:A13)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E15" t="e" cm="1">
+        <f t="array" aca="1" ref="E15" ca="1">su(B11:B13)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="13">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="e">
+        <f>200/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E16" t="e">
+        <f>300/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="13">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="17" t="e">
+        <f>D2+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E17" s="17" t="e">
+        <f>E2+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="13">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="e">
+        <f>EXP(D2*D2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E18" t="e">
+        <f>EXP(D2*D2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="13">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="e">
+        <f>LOOKUP("X",JAL:MAO)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E19" t="e">
+        <f>LOOKUP("X",JAM:MAP)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="13">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="e" vm="1">
+        <f>VLOOKUP(20,A:JAL,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E20" t="e" vm="1">
+        <f>VLOOKUP(20,A:B,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="13">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="e">
+        <f>A1 A2</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="E21" t="e">
+        <f>B1 B2</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="F21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="13">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="D22" ca="1">A:B</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E22" t="e" cm="1" vm="2">
+        <f t="array" aca="1" ref="E22" ca="1">A:B</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352FDB28-344C-5949-88B7-08D47DE77832}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A1:XFD23"/>
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="13"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="14">
+        <v>123456789.89</v>
+      </c>
+      <c r="E2">
+        <v>0.01</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>150</v>
+      </c>
+      <c r="E3">
+        <v>2.22333444555666E+20</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="G3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.13399</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>1234.5689</v>
+      </c>
+      <c r="E5">
+        <v>-2.0000000000000001E-4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="G5">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="15">
+        <v>44652</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.80233796296296289</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.52708333333333335</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G7">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>-890</v>
+      </c>
+      <c r="E8">
+        <v>-9800</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="G9">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="13">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="G10">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F11" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="G11">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="13">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="10">
+        <v>44562</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0.17708333333333334</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G13">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F14" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G14">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="13">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="b">
+        <f>IF(5=25/5,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="E15" t="b">
+        <f>"A"="A"</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="G15">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="13">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="b">
+        <f>0="A"</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G16">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="13">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="e" cm="1">
+        <f t="array" aca="1" ref="D17" ca="1">su(A12:A15)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E17" t="e" cm="1">
+        <f t="array" aca="1" ref="E17" ca="1">su(B12:B15)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="G17">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="13">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="e">
+        <f>200/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E18" t="e">
+        <f>300/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="G18">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="13">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="17" t="e">
+        <f>D2+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E19" s="17" t="e">
+        <f>E2+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="G19">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="13">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="e">
+        <f>EXP(D2*D2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E20" t="e">
+        <f>EXP(D2*D2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G20">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="13">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="e">
+        <f>LOOKUP("X",JAM:MAP)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E21" t="e">
+        <f>LOOKUP("X",JAN:MAQ)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="G21">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="13">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="e" vm="1">
+        <f>VLOOKUP(20,A:JAM,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E22" t="e" vm="1">
+        <f>VLOOKUP(20,A:B,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="13">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="e">
+        <f>A1 A2</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="E23" t="e">
+        <f>B1 B2</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="G23">
+        <v>1.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C990CE7E-915A-3241-9A9E-1ECC34525E61}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,7 +1804,7 @@
     <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -760,7 +1824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -777,7 +1841,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -794,7 +1858,7 @@
         <v>2.22333444555666E+20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -811,7 +1875,7 @@
         <v>0.13399</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -828,7 +1892,7 @@
         <v>-2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -845,7 +1909,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -861,8 +1925,12 @@
       <c r="E7" s="2">
         <v>0.52708333333333335</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>0.8</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -879,7 +1947,7 @@
         <v>-9800</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -893,7 +1961,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -910,492 +1978,31 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="13">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="10">
+        <v>44562</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="10">
-        <v>44562</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="11">
-        <v>0.17708333333333334</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="13">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="b">
-        <f>IF(5=25/5,TRUE,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="E15" t="b">
-        <f>"A"="A"</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="13">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" t="b">
-        <f>0="A"</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="13">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" t="e" cm="1">
-        <f t="array" aca="1" ref="D17" ca="1">su(A12:A15)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E17" t="e" cm="1">
-        <f t="array" aca="1" ref="E17" ca="1">su(B12:B15)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="13">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" t="e">
-        <f>200/0</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E18" t="e">
-        <f>300/0</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="13">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="17" t="e">
-        <f>D2+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E19" s="17" t="e">
-        <f>E2+#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="13">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" t="e">
-        <f>EXP(D2*D2)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E20" t="e">
-        <f>EXP(D2*D2)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="13">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" t="e">
-        <f>LOOKUP("X",JAM:MAP)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E21" t="e">
-        <f>LOOKUP("X",JAN:MAQ)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="13">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" t="e" vm="1">
-        <f>VLOOKUP(20,A:JAM,0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E22" t="e" vm="1">
-        <f>VLOOKUP(20,A:B,0)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="13">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" t="e">
-        <f>A1 A2</f>
-        <v>#NULL!</v>
-      </c>
-      <c r="E23" t="e">
-        <f>B1 B2</f>
-        <v>#NULL!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A24" s="13">
-        <v>13</v>
-      </c>
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A25" s="13">
-        <v>10</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA93BC24-192B-C24A-B2B9-6C19BFA160A2}">
-  <dimension ref="A1:F21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="13">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="18">
-        <v>123456789.89</v>
-      </c>
-      <c r="E2">
-        <v>0.01</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="13">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>150</v>
-      </c>
-      <c r="E3">
-        <v>2.22333444555666E+20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="E4" s="19">
-        <v>0.13399</v>
-      </c>
-      <c r="F4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="13">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>1234.5689</v>
-      </c>
-      <c r="E5">
-        <v>-2.0000000000000001E-4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="13">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="15">
-        <v>44652</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="13">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="16">
-        <v>0.80233796296296289</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.52708333333333335</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="13">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>-890</v>
-      </c>
-      <c r="E8">
-        <v>-9800</v>
-      </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="13">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="13">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="13">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="10">
-        <v>44562</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="13">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
@@ -1404,11 +2011,8 @@
       <c r="E12" s="11">
         <v>0.17708333333333334</v>
       </c>
-      <c r="F12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>14</v>
       </c>
@@ -1426,11 +2030,8 @@
         <f>"A"="A"</f>
         <v>1</v>
       </c>
-      <c r="F13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <v>15</v>
       </c>
@@ -1447,11 +2048,8 @@
         <f>0="A"</f>
         <v>0</v>
       </c>
-      <c r="F14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="13">
         <v>16</v>
       </c>
@@ -1469,11 +2067,8 @@
         <f t="array" aca="1" ref="E15" ca="1">su(B11:B13)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
         <v>17</v>
       </c>
@@ -1491,11 +2086,8 @@
         <f>300/0</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
         <v>18</v>
       </c>
@@ -1513,11 +2105,8 @@
         <f>E2+#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="F17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>19</v>
       </c>
@@ -1535,11 +2124,8 @@
         <f>EXP(D2*D2)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
         <v>20</v>
       </c>
@@ -1550,18 +2136,15 @@
         <v>37</v>
       </c>
       <c r="D19" t="e">
-        <f>LOOKUP("X",JAL:MAO)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E19" t="e">
         <f>LOOKUP("X",JAM:MAP)</f>
         <v>#N/A</v>
       </c>
-      <c r="F19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E19" t="e">
+        <f>LOOKUP("X",JAN:MAQ)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
         <v>21</v>
       </c>
@@ -1572,18 +2155,15 @@
         <v>38</v>
       </c>
       <c r="D20" t="e" vm="1">
-        <f>VLOOKUP(20,A:JAL,0)</f>
+        <f>VLOOKUP(20,A:JAM,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="E20" t="e" vm="1">
         <f>VLOOKUP(20,A:B,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="13">
         <v>22</v>
       </c>
@@ -1601,8 +2181,39 @@
         <f>B1 B2</f>
         <v>#NULL!</v>
       </c>
-      <c r="F21" t="s">
-        <v>40</v>
+    </row>
+    <row r="22" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A22" s="13">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" s="13">
+        <v>10</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>